<commit_message>
restructure/pipeline for multifeature linear regression
</commit_message>
<xml_diff>
--- a/Data/Economic_Indicators.xlsx
+++ b/Data/Economic_Indicators.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20359"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\2020_1\NLPython\Proj\CS372_Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016a41a89abc5981/2020_1/NLPython/Proj/CS372_Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_4B16120C1B2B2639604E90DC4BAF67173EAA9092" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D13725F1-611A-4B76-9B4B-20B05D163E9E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>YEAR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,11 +34,19 @@
     <t>GDP_GROWTH(%)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>UNEMPLOYMENT(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Export value index (2000 = 100)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,9 +86,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -360,489 +376,811 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B59"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1961</v>
       </c>
       <c r="B2">
         <v>2.2999999999996801</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
+        <v>6.6999998092651403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1962</v>
       </c>
       <c r="B3">
         <v>6.1000000000001204</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1963</v>
       </c>
       <c r="B4">
         <v>4.3999999999999204</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>5.6999998092651403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1964</v>
       </c>
       <c r="B5">
         <v>5.8000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>5.1999998092651403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1965</v>
       </c>
       <c r="B6">
         <v>6.3999999999997597</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1966</v>
       </c>
       <c r="B7">
         <v>6.5000000000002798</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>3.7999999523162802</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1967</v>
       </c>
       <c r="B8">
         <v>2.5000000000000302</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>3.7999999523162802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1968</v>
       </c>
       <c r="B9">
         <v>4.7999999999995904</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>3.5999999046325701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1969</v>
       </c>
       <c r="B10">
         <v>3.0999999999999899</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1970</v>
       </c>
       <c r="B11">
         <v>-0.254079592763304</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <v>4.9000000953674299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1971</v>
       </c>
       <c r="B12">
         <v>3.2933623777714298</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <v>5.9000000953674299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1972</v>
       </c>
       <c r="B13">
         <v>5.25889535776155</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <v>5.5999999046325701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1973</v>
       </c>
       <c r="B14">
         <v>5.64571947037473</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <v>4.9000000953674299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1974</v>
       </c>
       <c r="B15">
         <v>-0.54054652907490197</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <v>5.5999999046325701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1975</v>
       </c>
       <c r="B16">
         <v>-0.20546401213420001</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1976</v>
       </c>
       <c r="B17">
         <v>5.38813922657351</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <v>7.6999998092651403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1977</v>
       </c>
       <c r="B18">
         <v>4.6241592068368904</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1">
+        <v>7.0999999046325701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1978</v>
       </c>
       <c r="B19">
         <v>5.5353026932853302</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
+        <v>6.0999999046325701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1979</v>
       </c>
       <c r="B20">
         <v>3.1661502709532101</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <v>5.8000001907348597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1980</v>
       </c>
       <c r="B21">
         <v>-0.256751930992138</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C21" s="1">
+        <v>31.375502730000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7.0999999046325701</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1981</v>
       </c>
       <c r="B22">
         <v>2.5377186978074602</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C22" s="1">
+        <v>30.85024263</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7.5999999046325701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1982</v>
       </c>
       <c r="B23">
         <v>-1.8028744527117599</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C23" s="1">
+        <v>29.251601569999998</v>
+      </c>
+      <c r="D23" s="1">
+        <v>9.6999998092651403</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1983</v>
       </c>
       <c r="B24">
         <v>4.5839273156610103</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C24" s="1">
+        <v>28.971391409999999</v>
+      </c>
+      <c r="D24" s="1">
+        <v>9.6000003814697301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1984</v>
       </c>
       <c r="B25">
         <v>7.23661999357385</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C25" s="1">
+        <v>30.830603270000001</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1985</v>
       </c>
       <c r="B26">
         <v>4.1696559543024296</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C26" s="1">
+        <v>31.826555949999999</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7.1999998092651403</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1986</v>
       </c>
       <c r="B27">
         <v>3.46265171279892</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C27" s="1">
+        <v>36.779226860000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1987</v>
       </c>
       <c r="B28">
         <v>3.4595725553488301</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C28" s="1">
+        <v>42.854095370000003</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6.1999998092651403</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1988</v>
       </c>
       <c r="B29">
         <v>4.1770463844437797</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C29" s="1">
+        <v>48.863048310000003</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1989</v>
       </c>
       <c r="B30">
         <v>3.6726563285104601</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C30" s="1">
+        <v>52.054800239999999</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5.3000001907348597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1990</v>
       </c>
       <c r="B31">
         <v>1.8859603230941799</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C31" s="1">
+        <v>59.508545929999997</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5.5999999046325701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1991</v>
       </c>
       <c r="B32">
         <v>-0.108259105278663</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C32" s="1">
+        <v>60.403948030000002</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6.8000001907348597</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1992</v>
       </c>
       <c r="B33">
         <v>3.52244249386644</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C33" s="1">
+        <v>64.159120229999999</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1993</v>
       </c>
       <c r="B34">
         <v>2.7528443268801199</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C34" s="1">
+        <v>63.133465289999997</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6.9000000953674299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1994</v>
       </c>
       <c r="B35">
         <v>4.0288390635428</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C35" s="1">
+        <v>71.251752280000005</v>
+      </c>
+      <c r="D35" s="1">
+        <v>6.1187000274658203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1995</v>
       </c>
       <c r="B36">
         <v>2.6842871324197701</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C36" s="1">
+        <v>74.783161410000005</v>
+      </c>
+      <c r="D36" s="1">
+        <v>5.6504001617431596</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1996</v>
       </c>
       <c r="B37">
         <v>3.7725013192651899</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C37" s="1">
+        <v>79.940991249999996</v>
+      </c>
+      <c r="D37" s="1">
+        <v>5.4510998725891104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1997</v>
       </c>
       <c r="B38">
         <v>4.4472163427340803</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C38" s="1">
+        <v>88.139932830000006</v>
+      </c>
+      <c r="D38" s="1">
+        <v>5.0002999305725098</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1998</v>
       </c>
       <c r="B39">
         <v>4.48140755451207</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C39" s="1">
+        <v>87.239071100000004</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4.5104999542236301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1999</v>
       </c>
       <c r="B40">
         <v>4.7532359887971696</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C40" s="1">
+        <v>88.985929470000002</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4.2188000679016104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2000</v>
       </c>
       <c r="B41">
         <v>4.1274840135585302</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C41" s="1">
+        <v>100</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3.9920001029968302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2001</v>
       </c>
       <c r="B42">
         <v>0.99834079465650005</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C42" s="1">
+        <v>93.245071730000006</v>
+      </c>
+      <c r="D42" s="1">
+        <v>4.7312998771667498</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2002</v>
       </c>
       <c r="B43">
         <v>1.7416952497297999</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C43" s="1">
+        <v>88.641392060000001</v>
+      </c>
+      <c r="D43" s="1">
+        <v>5.7831997871398899</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2003</v>
       </c>
       <c r="B44">
         <v>2.8612107674102401</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C44" s="1">
+        <v>92.691433119999999</v>
+      </c>
+      <c r="D44" s="1">
+        <v>5.9886999130248997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2004</v>
       </c>
       <c r="B45">
         <v>3.7988911266239298</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C45" s="1">
+        <v>104.2148921</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5.5286002159118697</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2005</v>
       </c>
       <c r="B46">
         <v>3.5132137966530199</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C46" s="1">
+        <v>115.2399612</v>
+      </c>
+      <c r="D46" s="1">
+        <v>5.0834999084472701</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2006</v>
       </c>
       <c r="B47">
         <v>2.8549722917001499</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C47" s="1">
+        <v>131.2115848</v>
+      </c>
+      <c r="D47" s="1">
+        <v>4.6230001449584996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2007</v>
       </c>
       <c r="B48">
         <v>1.87617145846693</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C48" s="1">
+        <v>146.84391460000001</v>
+      </c>
+      <c r="D48" s="1">
+        <v>4.6220998764038104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2008</v>
       </c>
       <c r="B49">
         <v>-0.136579805460741</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C49" s="1">
+        <v>164.65179209999999</v>
+      </c>
+      <c r="D49" s="1">
+        <v>5.7842001914978001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2009</v>
       </c>
       <c r="B50">
         <v>-2.5367570658566501</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C50" s="1">
+        <v>135.05802399999999</v>
+      </c>
+      <c r="D50" s="1">
+        <v>9.2541999816894496</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2010</v>
       </c>
       <c r="B51">
         <v>2.5637665587658098</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C51" s="1">
+        <v>163.5075545</v>
+      </c>
+      <c r="D51" s="1">
+        <v>9.6333999633789098</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2011</v>
       </c>
       <c r="B52">
         <v>1.5508355056815599</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C52" s="1">
+        <v>189.5989093</v>
+      </c>
+      <c r="D52" s="1">
+        <v>8.9491996765136701</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2012</v>
       </c>
       <c r="B53">
         <v>2.2495458523699199</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C53" s="1">
+        <v>197.68095890000001</v>
+      </c>
+      <c r="D53" s="1">
+        <v>8.0693998336791992</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2013</v>
       </c>
       <c r="B54">
         <v>1.84208107101102</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C54" s="1">
+        <v>202.0151602</v>
+      </c>
+      <c r="D54" s="1">
+        <v>7.37489986419678</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2014</v>
       </c>
       <c r="B55">
         <v>2.4519730353603402</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C55" s="1">
+        <v>207.25087540000001</v>
+      </c>
+      <c r="D55" s="1">
+        <v>6.1675000190734899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2015</v>
       </c>
       <c r="B56">
         <v>2.8809104660521898</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C56" s="1">
+        <v>192.1649329</v>
+      </c>
+      <c r="D56" s="1">
+        <v>5.2800002098083496</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2016</v>
       </c>
       <c r="B57">
         <v>1.5672151699786401</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C57" s="1">
+        <v>185.57069920000001</v>
+      </c>
+      <c r="D57" s="1">
+        <v>4.8692002296447798</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2017</v>
       </c>
       <c r="B58">
         <v>2.21701033031884</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C58" s="1">
+        <v>197.75385650000001</v>
+      </c>
+      <c r="D58" s="1">
+        <v>4.3551998138427699</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2018</v>
       </c>
       <c r="B59">
         <v>2.92732272821085</v>
+      </c>
+      <c r="C59" s="1">
+        <v>213.06479709999999</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3.8956000804901101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="1">
+        <v>3.66919994354248</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
plugging in new keyword group
</commit_message>
<xml_diff>
--- a/Data/Economic_Indicators.xlsx
+++ b/Data/Economic_Indicators.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016a41a89abc5981/2020_1/NLPython/Proj/CS372_Project/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y\OneDrive\2020_1\NLPython\Proj\CS372_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_4B16120C1B2B2639604E90DC4BAF67173EAA9092" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D13725F1-611A-4B76-9B4B-20B05D163E9E}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_4B16120C1B2B2639604E90DC4BAF67173EAA9092" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{275BE869-26B8-4CED-A60D-9D189E7C28F1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,15 +31,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GDP_GROWTH(%)</t>
+    <t>GDP_GROWTH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UNEMPLOYMENT(%)</t>
+    <t>EXPORT_INDEX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Export value index (2000 = 100)</t>
+    <t>UNEMPLOYMENT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -380,12 +380,12 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,10 +393,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>